<commit_message>
adapt for mail adress column
</commit_message>
<xml_diff>
--- a/test/Contactsheet.xlsx
+++ b/test/Contactsheet.xlsx
@@ -277,10 +277,10 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.40625" defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.41796875" defaultRowHeight="15.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.1"/>

</xml_diff>